<commit_message>
updated test metadata file
</commit_message>
<xml_diff>
--- a/test/test_metadata.xlsx
+++ b/test/test_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdstengl/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vir5\ONEDRI~1\MobaXterm\slash\RemoteFiles\394900_6_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949A22BC-6102-154C-AA2A-9CA71C5E41EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677AEF40-34B1-42BB-BE6E-4693518030C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{D5FDF35F-C226-47A5-9BF2-786F5A743106}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{D5FDF35F-C226-47A5-9BF2-786F5A743106}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,35 +32,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
-  <si>
-    <t>State</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>Index</t>
   </si>
   <si>
-    <t>vial</t>
-  </si>
-  <si>
     <t>adult</t>
   </si>
   <si>
-    <t>Dermacentor andersoni</t>
-  </si>
-  <si>
-    <t>PC</t>
-  </si>
-  <si>
-    <t>iPM3</t>
-  </si>
-  <si>
     <t>Submission_No</t>
   </si>
   <si>
-    <t>Vial_ID</t>
-  </si>
-  <si>
     <t>Pathogen_Testing_ID</t>
   </si>
   <si>
@@ -91,9 +73,6 @@
     <t>Borrelia_miyamotoi</t>
   </si>
   <si>
-    <t>pathogen_pos</t>
-  </si>
-  <si>
     <t>I_pacificus</t>
   </si>
   <si>
@@ -106,84 +85,33 @@
     <t>D_andersoni</t>
   </si>
   <si>
-    <t>NC21_0017</t>
-  </si>
-  <si>
-    <t>NC21-Ticks_17-110</t>
-  </si>
-  <si>
     <t>A-01</t>
   </si>
   <si>
     <t>AK2019_1</t>
   </si>
   <si>
-    <t>Ixodes pacificus</t>
-  </si>
-  <si>
     <t>AK2019_20</t>
   </si>
   <si>
-    <t>Dermacentor variabilis</t>
-  </si>
-  <si>
     <t>AK2019_11</t>
   </si>
   <si>
-    <t>Plate_Position</t>
-  </si>
-  <si>
-    <t>Plate_Label</t>
-  </si>
-  <si>
-    <t>Rerun</t>
-  </si>
-  <si>
-    <t>Date_of_Collection</t>
-  </si>
-  <si>
-    <t>Study_type</t>
-  </si>
-  <si>
-    <t>Sample_Type</t>
-  </si>
-  <si>
-    <t>Tick_Sex</t>
-  </si>
-  <si>
     <t>Morphological_Ectoparasite_Genus_Species</t>
   </si>
   <si>
     <t>Lifestage</t>
   </si>
   <si>
-    <t>Host_Genus_Species</t>
-  </si>
-  <si>
     <t>County</t>
   </si>
   <si>
     <t>Site</t>
   </si>
   <si>
-    <t>Date_Library_Prep</t>
-  </si>
-  <si>
-    <t>Date_Illumina_Run</t>
-  </si>
-  <si>
-    <t>Illumina _MM</t>
-  </si>
-  <si>
-    <t>Illumina_Kit</t>
-  </si>
-  <si>
     <t>batch</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -208,9 +136,6 @@
     <t>Control_Borrelia_miyamotoi</t>
   </si>
   <si>
-    <t>Control_pathogen_pos</t>
-  </si>
-  <si>
     <t>Control_empty_fastq</t>
   </si>
   <si>
@@ -224,6 +149,33 @@
   </si>
   <si>
     <t>Control_NC</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -272,7 +224,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -314,19 +266,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -342,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -357,9 +296,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -680,317 +616,284 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B0CF52-72C2-41C0-80A7-09E8477A6B92}">
-  <dimension ref="A1:Y10"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" customWidth="1"/>
-    <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" customWidth="1"/>
-    <col min="12" max="12" width="28.33203125" customWidth="1"/>
-    <col min="16" max="16" width="33.83203125" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="J3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" t="s">
         <v>39</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" t="s">
-        <v>50</v>
-      </c>
-      <c r="P2" t="s">
-        <v>59</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" t="s">
-        <v>51</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="7">
-        <v>96</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="U6" t="s">
-        <v>6</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" t="s">
-        <v>52</v>
-      </c>
-      <c r="N7" t="s">
-        <v>3</v>
-      </c>
-      <c r="O7" t="s">
-        <v>28</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="U7" t="s">
-        <v>6</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="7">
-        <v>5</v>
-      </c>
-      <c r="G8" t="s">
-        <v>2</v>
-      </c>
-      <c r="M8" t="s">
-        <v>53</v>
-      </c>
-      <c r="N8" t="s">
-        <v>3</v>
-      </c>
-      <c r="O8" t="s">
-        <v>4</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="U8" t="s">
-        <v>6</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y8" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="7">
-        <v>9</v>
-      </c>
-      <c r="G9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9" t="s">
-        <v>54</v>
-      </c>
-      <c r="N9" t="s">
-        <v>3</v>
-      </c>
-      <c r="O9" t="s">
-        <v>30</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="U9" t="s">
-        <v>6</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y9" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="7">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M10" t="s">
-        <v>51</v>
-      </c>
-      <c r="N10" t="s">
-        <v>51</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="U10" t="s">
-        <v>6</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y10" s="1">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated test metadata file with state column
</commit_message>
<xml_diff>
--- a/test/test_metadata.xlsx
+++ b/test/test_metadata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vir5\ONEDRI~1\MobaXterm\slash\RemoteFiles\394900_6_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vir5\ONEDRI~1\MobaXterm\slash\RemoteFiles\394900_6_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677AEF40-34B1-42BB-BE6E-4693518030C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F10D648-7C05-4518-AD54-99D0DBF491D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{D5FDF35F-C226-47A5-9BF2-786F5A743106}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>County</t>
   </si>
   <si>
-    <t>Site</t>
-  </si>
-  <si>
     <t>batch</t>
   </si>
   <si>
@@ -176,6 +173,9 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>State</t>
   </si>
 </sst>
 </file>
@@ -619,7 +619,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,7 +632,7 @@
     <col min="9" max="9" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -655,13 +655,13 @@
         <v>23</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -669,28 +669,28 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -698,28 +698,28 @@
         <v>6</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -727,28 +727,28 @@
         <v>6</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -756,28 +756,28 @@
         <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -785,28 +785,28 @@
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -814,28 +814,28 @@
         <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -843,28 +843,28 @@
         <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -872,28 +872,28 @@
         <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new test datasets with 5, 10, or 25 reads.  Relates to issue #100
</commit_message>
<xml_diff>
--- a/test/test_metadata.xlsx
+++ b/test/test_metadata.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vir5\ONEDRI~1\MobaXterm\slash\RemoteFiles\394900_6_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdstengl/Library/Caches/com.binarynights.ForkLift/FileCache/91EE7E3E-57D0-462E-BFE1-9326C9FF9847/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F10D648-7C05-4518-AD54-99D0DBF491D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31313B1A-6CD9-E344-A511-923A3315A07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{D5FDF35F-C226-47A5-9BF2-786F5A743106}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25440" windowHeight="15400" xr2:uid="{D5FDF35F-C226-47A5-9BF2-786F5A743106}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="57">
   <si>
     <t>Index</t>
   </si>
@@ -157,25 +157,52 @@
     <t>c</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
     <t>f</t>
   </si>
   <si>
-    <t>g</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>h</t>
-  </si>
-  <si>
     <t>State</t>
+  </si>
+  <si>
+    <t>Control_Borrelia_burgdoreri_B31_5</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Borrelia_burgdoreri_B31_5</t>
+  </si>
+  <si>
+    <t>Control_Borrelia_burgdoreri_B31_10</t>
+  </si>
+  <si>
+    <t>Borrelia_burgdoreri_B31_10</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>Control_Borrelia_burgdoreri_B31_25</t>
+  </si>
+  <si>
+    <t>Borrelia_burgdoreri_B31_25</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
 </sst>
 </file>
@@ -320,9 +347,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -360,7 +387,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -466,7 +493,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -608,7 +635,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -616,23 +643,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B0CF52-72C2-41C0-80A7-09E8477A6B92}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -655,7 +682,7 @@
         <v>23</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>0</v>
@@ -664,7 +691,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -681,10 +708,10 @@
         <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>9</v>
@@ -693,7 +720,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -710,10 +737,10 @@
         <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>10</v>
@@ -722,7 +749,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -739,10 +766,10 @@
         <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
@@ -751,148 +778,235 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
         <v>45</v>
       </c>
-      <c r="H5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="J8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
         <v>27</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F9" t="s">
         <v>1</v>
       </c>
-      <c r="G6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="J9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
         <v>28</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F10" t="s">
         <v>1</v>
       </c>
-      <c r="G7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="J10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" t="s">
         <v>29</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F11" t="s">
         <v>1</v>
       </c>
-      <c r="G8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="J11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J12" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>